<commit_message>
Introduction update.. continued.. no built
</commit_message>
<xml_diff>
--- a/data/02_data_extraction/data_extraction_setSD_checkedTR.xlsx
+++ b/data/02_data_extraction/data_extraction_setSD_checkedTR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/GNM_Analysis/data/02_data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Desktop/Green_Nest_Material/data/02_data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBCD8E6-76D2-944B-995C-7B97C8844FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E10132-00A5-4844-B070-15BDE24D7643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="500" windowWidth="62660" windowHeight="21100" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
+    <workbookView xWindow="-49540" yWindow="-21500" windowWidth="42440" windowHeight="26040" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -1144,9 +1144,6 @@
     <t xml:space="preserve">We expect a negative relationship between telomere dynamic and GNM. Telomere dynamic is calculated as rank difference in telomere length. </t>
   </si>
   <si>
-    <t>Authors say that the adults from green material would be with better body condition as compared to those without the green nest material. If they are healthier, they could provide better parental care to the nestlings.</t>
-  </si>
-  <si>
     <t>Authors say: Spotless starling females generally removed the green nesting material, both the experimental plants added by the researchers and those put into the nests by the males. I have given an NA for this considering the experimental nests are not blank and could have a mix of aromatic plants still in the control group.</t>
   </si>
   <si>
@@ -1186,6 +1183,9 @@
   </si>
   <si>
     <t>sensitivity-analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors are just using female body condition to control for the effect it can have. We are excluding it and adult body condition being affected by GNM is rather tricky to interpret and describe a true direction of effect for. </t>
   </si>
 </sst>
 </file>
@@ -1769,9 +1769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCDDD25-569C-114E-BA1C-CFE63559CC31}">
   <dimension ref="A1:AX119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD63" sqref="AD63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD78" sqref="AD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1956,10 +1956,10 @@
         <v>105</v>
       </c>
       <c r="AW1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="AX1" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:50" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2963,7 +2963,7 @@
         <v>275</v>
       </c>
       <c r="AD8" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AE8" s="9">
         <v>-1</v>
@@ -3419,7 +3419,7 @@
         <v>275</v>
       </c>
       <c r="AD11" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AE11" s="9">
         <v>-1</v>
@@ -7368,10 +7368,10 @@
         <v>181</v>
       </c>
       <c r="AC37" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AD37" s="8" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="AE37" s="9">
         <v>1</v>
@@ -7520,10 +7520,10 @@
         <v>181</v>
       </c>
       <c r="AC38" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AD38" s="8" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="AE38" s="9">
         <v>1</v>
@@ -11323,7 +11323,7 @@
         <v>275</v>
       </c>
       <c r="AD63" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE63" s="5">
         <v>1</v>
@@ -11475,7 +11475,7 @@
         <v>275</v>
       </c>
       <c r="AD64" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE64" s="5">
         <v>1</v>
@@ -11627,7 +11627,7 @@
         <v>275</v>
       </c>
       <c r="AD65" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE65" s="5">
         <v>1</v>
@@ -11779,7 +11779,7 @@
         <v>275</v>
       </c>
       <c r="AD66" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE66" s="5">
         <v>-1</v>
@@ -11931,7 +11931,7 @@
         <v>275</v>
       </c>
       <c r="AD67" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE67" s="5">
         <v>-1</v>
@@ -12083,7 +12083,7 @@
         <v>275</v>
       </c>
       <c r="AD68" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE68" s="5">
         <v>-1</v>
@@ -12235,7 +12235,7 @@
         <v>275</v>
       </c>
       <c r="AD69" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE69" s="5">
         <v>-1</v>
@@ -12387,7 +12387,7 @@
         <v>275</v>
       </c>
       <c r="AD70" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE70" s="5">
         <v>-1</v>
@@ -12539,7 +12539,7 @@
         <v>275</v>
       </c>
       <c r="AD71" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE71" s="5">
         <v>-1</v>
@@ -12730,7 +12730,7 @@
         <v>109</v>
       </c>
       <c r="AQ72" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR72" s="11" t="s">
         <v>111</v>
@@ -12882,7 +12882,7 @@
         <v>109</v>
       </c>
       <c r="AQ73" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR73" s="11" t="s">
         <v>111</v>
@@ -13034,7 +13034,7 @@
         <v>109</v>
       </c>
       <c r="AQ74" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR74" s="11" t="s">
         <v>111</v>
@@ -13144,7 +13144,7 @@
         <v>181</v>
       </c>
       <c r="AC75" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AD75" s="9" t="s">
         <v>292</v>
@@ -13186,7 +13186,7 @@
         <v>109</v>
       </c>
       <c r="AQ75" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR75" s="11" t="s">
         <v>111</v>
@@ -13296,7 +13296,7 @@
         <v>181</v>
       </c>
       <c r="AC76" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AD76" s="9" t="s">
         <v>292</v>
@@ -13338,7 +13338,7 @@
         <v>109</v>
       </c>
       <c r="AQ76" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR76" s="11" t="s">
         <v>111</v>
@@ -13448,7 +13448,7 @@
         <v>181</v>
       </c>
       <c r="AC77" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AD77" s="9" t="s">
         <v>292</v>
@@ -13490,7 +13490,7 @@
         <v>109</v>
       </c>
       <c r="AQ77" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AR77" s="11" t="s">
         <v>111</v>
@@ -13603,7 +13603,7 @@
         <v>275</v>
       </c>
       <c r="AD78" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE78" s="5">
         <v>1</v>
@@ -13755,7 +13755,7 @@
         <v>275</v>
       </c>
       <c r="AD79" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE79" s="5">
         <v>1</v>
@@ -13907,7 +13907,7 @@
         <v>275</v>
       </c>
       <c r="AD80" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE80" s="5">
         <v>1</v>
@@ -14059,7 +14059,7 @@
         <v>275</v>
       </c>
       <c r="AD81" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE81" s="5">
         <v>1</v>
@@ -14211,7 +14211,7 @@
         <v>275</v>
       </c>
       <c r="AD82" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE82" s="5">
         <v>1</v>
@@ -14363,7 +14363,7 @@
         <v>275</v>
       </c>
       <c r="AD83" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE83" s="5">
         <v>1</v>
@@ -14515,7 +14515,7 @@
         <v>275</v>
       </c>
       <c r="AD84" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE84" s="5">
         <v>1</v>
@@ -14667,7 +14667,7 @@
         <v>275</v>
       </c>
       <c r="AD85" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE85" s="5">
         <v>1</v>
@@ -14819,7 +14819,7 @@
         <v>275</v>
       </c>
       <c r="AD86" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE86" s="5">
         <v>1</v>
@@ -14971,7 +14971,7 @@
         <v>275</v>
       </c>
       <c r="AD87" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE87" s="5">
         <v>1</v>
@@ -15123,7 +15123,7 @@
         <v>275</v>
       </c>
       <c r="AD88" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE88" s="5">
         <v>1</v>
@@ -15275,7 +15275,7 @@
         <v>275</v>
       </c>
       <c r="AD89" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE89" s="5">
         <v>1</v>
@@ -15427,7 +15427,7 @@
         <v>275</v>
       </c>
       <c r="AD90" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE90" s="5">
         <v>1</v>
@@ -15579,7 +15579,7 @@
         <v>275</v>
       </c>
       <c r="AD91" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE91" s="5">
         <v>1</v>
@@ -15731,7 +15731,7 @@
         <v>275</v>
       </c>
       <c r="AD92" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE92" s="5">
         <v>1</v>
@@ -15883,7 +15883,7 @@
         <v>275</v>
       </c>
       <c r="AD93" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE93" s="5">
         <v>1</v>
@@ -16035,7 +16035,7 @@
         <v>275</v>
       </c>
       <c r="AD94" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE94" s="5">
         <v>1</v>
@@ -16187,7 +16187,7 @@
         <v>275</v>
       </c>
       <c r="AD95" s="37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE95" s="5">
         <v>1</v>
@@ -16303,7 +16303,7 @@
         <v>42.85</v>
       </c>
       <c r="R96" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S96" s="8" t="s">
         <v>108</v>
@@ -16318,7 +16318,7 @@
         <v>15.38</v>
       </c>
       <c r="W96" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X96" s="8" t="s">
         <v>108</v>
@@ -16336,10 +16336,10 @@
         <v>153</v>
       </c>
       <c r="AC96" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD96" s="33" t="s">
         <v>301</v>
-      </c>
-      <c r="AD96" s="33" t="s">
-        <v>302</v>
       </c>
       <c r="AE96" s="9">
         <v>1</v>
@@ -16455,7 +16455,7 @@
         <v>15.38</v>
       </c>
       <c r="R97" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S97" s="8" t="s">
         <v>108</v>
@@ -16470,7 +16470,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="W97" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X97" s="8" t="s">
         <v>108</v>
@@ -16488,10 +16488,10 @@
         <v>153</v>
       </c>
       <c r="AC97" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD97" s="33" t="s">
         <v>301</v>
-      </c>
-      <c r="AD97" s="33" t="s">
-        <v>302</v>
       </c>
       <c r="AE97" s="9">
         <v>1</v>
@@ -16607,7 +16607,7 @@
         <v>42.85</v>
       </c>
       <c r="R98" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S98" s="8" t="s">
         <v>108</v>
@@ -16622,7 +16622,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="W98" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X98" s="8" t="s">
         <v>108</v>
@@ -16640,10 +16640,10 @@
         <v>153</v>
       </c>
       <c r="AC98" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD98" s="33" t="s">
         <v>301</v>
-      </c>
-      <c r="AD98" s="33" t="s">
-        <v>302</v>
       </c>
       <c r="AE98" s="9">
         <v>1</v>
@@ -19024,7 +19024,7 @@
         <v>250</v>
       </c>
       <c r="M114" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N114" s="10" t="s">
         <v>108</v>
@@ -19072,7 +19072,7 @@
         <v>153</v>
       </c>
       <c r="AC114" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD114" s="9" t="s">
         <v>290</v>
@@ -19114,7 +19114,7 @@
         <v>109</v>
       </c>
       <c r="AQ114" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR114" s="10" t="s">
         <v>111</v>
@@ -19176,7 +19176,7 @@
         <v>250</v>
       </c>
       <c r="M115" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N115" s="10" t="s">
         <v>108</v>
@@ -19224,7 +19224,7 @@
         <v>153</v>
       </c>
       <c r="AC115" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD115" s="9" t="s">
         <v>290</v>
@@ -19266,7 +19266,7 @@
         <v>109</v>
       </c>
       <c r="AQ115" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR115" s="10" t="s">
         <v>111</v>
@@ -19328,7 +19328,7 @@
         <v>250</v>
       </c>
       <c r="M116" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N116" s="10" t="s">
         <v>108</v>
@@ -19376,7 +19376,7 @@
         <v>153</v>
       </c>
       <c r="AC116" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD116" s="9" t="s">
         <v>290</v>
@@ -19418,7 +19418,7 @@
         <v>109</v>
       </c>
       <c r="AQ116" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR116" s="10" t="s">
         <v>111</v>
@@ -19480,7 +19480,7 @@
         <v>250</v>
       </c>
       <c r="M117" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N117" s="10" t="s">
         <v>108</v>
@@ -19528,7 +19528,7 @@
         <v>153</v>
       </c>
       <c r="AC117" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD117" s="9" t="s">
         <v>290</v>
@@ -19570,7 +19570,7 @@
         <v>109</v>
       </c>
       <c r="AQ117" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR117" s="10" t="s">
         <v>111</v>
@@ -19632,7 +19632,7 @@
         <v>250</v>
       </c>
       <c r="M118" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N118" s="10" t="s">
         <v>108</v>
@@ -19680,7 +19680,7 @@
         <v>153</v>
       </c>
       <c r="AC118" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD118" s="9" t="s">
         <v>290</v>
@@ -19722,7 +19722,7 @@
         <v>109</v>
       </c>
       <c r="AQ118" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR118" s="10" t="s">
         <v>111</v>
@@ -19784,7 +19784,7 @@
         <v>250</v>
       </c>
       <c r="M119" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N119" s="10" t="s">
         <v>108</v>
@@ -19832,7 +19832,7 @@
         <v>153</v>
       </c>
       <c r="AC119" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD119" s="9" t="s">
         <v>290</v>
@@ -19874,7 +19874,7 @@
         <v>109</v>
       </c>
       <c r="AQ119" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AR119" s="10" t="s">
         <v>111</v>

</xml_diff>